<commit_message>
Modify: Add W007 for ipr
</commit_message>
<xml_diff>
--- a/storage/app/iprs/1/week_2.xlsx
+++ b/storage/app/iprs/1/week_2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Smoku\Pfron\pfron-backend\storage\app\iprs\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23ACC6C3-DB80-4EDB-B698-E765ED3B8109}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA668085-E340-454D-9006-613A67230FCE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>id</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>M1-W049</t>
+  </si>
+  <si>
+    <t>M1-W007</t>
   </si>
 </sst>
 </file>
@@ -205,7 +208,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -239,6 +242,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF95B3D7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -328,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -363,6 +372,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -652,13 +673,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AMP48"/>
+  <dimension ref="A1:AMP49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AB2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A22" sqref="A22:XFD22"/>
+      <selection pane="bottomRight" activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1086,7 +1107,7 @@
       <c r="AN6" s="8"/>
       <c r="AO6" s="8"/>
     </row>
-    <row r="7" spans="1:41" ht="15.75" thickBot="1">
+    <row r="7" spans="1:41" ht="16.5" customHeight="1" thickBot="1">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -1157,84 +1178,92 @@
       <c r="AN7" s="8"/>
       <c r="AO7" s="8"/>
     </row>
-    <row r="8" spans="1:41" ht="15.75" thickBot="1">
-      <c r="A8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="9">
-        <v>2</v>
-      </c>
-      <c r="F8" s="9">
-        <v>2</v>
-      </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="10">
+    <row r="8" spans="1:41" ht="16.5" customHeight="1" thickBot="1">
+      <c r="A8" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="15">
+        <v>2</v>
+      </c>
+      <c r="F8" s="15">
+        <v>2</v>
+      </c>
+      <c r="G8" s="15">
+        <v>2</v>
+      </c>
+      <c r="H8" s="15">
+        <v>2</v>
+      </c>
+      <c r="I8" s="15">
+        <v>2</v>
+      </c>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="15">
+        <v>5</v>
+      </c>
+      <c r="N8" s="15">
+        <v>14</v>
+      </c>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="16">
+        <v>178</v>
+      </c>
+      <c r="R8" s="14"/>
+      <c r="S8" s="16">
         <v>4</v>
       </c>
-      <c r="N8" s="9">
-        <v>11</v>
-      </c>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="10">
-        <v>92</v>
-      </c>
-      <c r="R8" s="8"/>
-      <c r="S8" s="9">
-        <v>3</v>
-      </c>
-      <c r="T8" s="8"/>
-      <c r="U8" s="8"/>
-      <c r="V8" s="8"/>
-      <c r="W8" s="9">
-        <v>4</v>
-      </c>
-      <c r="X8" s="10">
-        <v>18</v>
-      </c>
-      <c r="Y8" s="8"/>
+      <c r="T8" s="14"/>
+      <c r="U8" s="14"/>
+      <c r="V8" s="16">
+        <v>0</v>
+      </c>
+      <c r="W8" s="15">
+        <v>3</v>
+      </c>
+      <c r="X8" s="15">
+        <v>6</v>
+      </c>
+      <c r="Y8" s="16">
+        <v>2</v>
+      </c>
       <c r="Z8" s="12"/>
-      <c r="AA8" s="9">
-        <v>5</v>
-      </c>
-      <c r="AB8" s="8"/>
-      <c r="AC8" s="8"/>
-      <c r="AD8" s="8"/>
-      <c r="AE8" s="9">
-        <v>52</v>
-      </c>
-      <c r="AF8" s="10">
-        <v>66</v>
-      </c>
-      <c r="AG8" s="8"/>
-      <c r="AH8" s="10">
-        <v>0</v>
-      </c>
-      <c r="AI8" s="8"/>
-      <c r="AJ8" s="10">
-        <v>91</v>
-      </c>
-      <c r="AK8" s="9">
-        <v>85.5</v>
-      </c>
-      <c r="AL8" s="8"/>
-      <c r="AM8" s="9">
-        <v>5</v>
-      </c>
-      <c r="AN8" s="8"/>
-      <c r="AO8" s="8"/>
+      <c r="AA8" s="15">
+        <v>3</v>
+      </c>
+      <c r="AB8" s="14"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="3"/>
+      <c r="AE8" s="16">
+        <v>42.5</v>
+      </c>
+      <c r="AF8" s="16">
+        <v>16</v>
+      </c>
+      <c r="AG8" s="14"/>
+      <c r="AH8" s="14"/>
+      <c r="AI8" s="14"/>
+      <c r="AJ8" s="16">
+        <v>67</v>
+      </c>
+      <c r="AK8" s="15">
+        <v>62.5</v>
+      </c>
+      <c r="AL8" s="14"/>
+      <c r="AM8" s="14"/>
+      <c r="AN8" s="14"/>
+      <c r="AO8" s="15">
+        <v>27</v>
+      </c>
     </row>
     <row r="9" spans="1:41" ht="15.75" thickBot="1">
       <c r="A9" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -1245,73 +1274,71 @@
       <c r="F9" s="9">
         <v>2</v>
       </c>
-      <c r="G9" s="9">
-        <v>2</v>
-      </c>
-      <c r="H9" s="9">
-        <v>2</v>
-      </c>
-      <c r="I9" s="9">
-        <v>2</v>
-      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
-      <c r="M9" s="9">
-        <v>2</v>
+      <c r="M9" s="10">
+        <v>4</v>
       </c>
       <c r="N9" s="9">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="O9" s="8"/>
       <c r="P9" s="8"/>
       <c r="Q9" s="10">
-        <v>178</v>
+        <v>92</v>
       </c>
       <c r="R9" s="8"/>
       <c r="S9" s="9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T9" s="8"/>
       <c r="U9" s="8"/>
       <c r="V9" s="8"/>
       <c r="W9" s="9">
-        <v>2</v>
-      </c>
-      <c r="X9" s="9">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="X9" s="10">
+        <v>18</v>
       </c>
       <c r="Y9" s="8"/>
       <c r="Z9" s="12"/>
       <c r="AA9" s="9">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AB9" s="8"/>
       <c r="AC9" s="8"/>
       <c r="AD9" s="8"/>
-      <c r="AE9" s="10">
-        <v>20.5</v>
-      </c>
-      <c r="AF9" s="9">
-        <v>6</v>
+      <c r="AE9" s="9">
+        <v>52</v>
+      </c>
+      <c r="AF9" s="10">
+        <v>66</v>
       </c>
       <c r="AG9" s="8"/>
-      <c r="AH9" s="8"/>
+      <c r="AH9" s="10">
+        <v>0</v>
+      </c>
       <c r="AI9" s="8"/>
       <c r="AJ9" s="10">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="AK9" s="9">
-        <v>59</v>
-      </c>
-      <c r="AL9" s="7"/>
-      <c r="AM9" s="7"/>
-      <c r="AN9" s="7"/>
+        <v>85.5</v>
+      </c>
+      <c r="AL9" s="8"/>
+      <c r="AM9" s="9">
+        <v>5</v>
+      </c>
+      <c r="AN9" s="8"/>
       <c r="AO9" s="8"/>
     </row>
     <row r="10" spans="1:41" ht="15.75" thickBot="1">
       <c r="A10" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -1338,39 +1365,39 @@
         <v>2</v>
       </c>
       <c r="N10" s="9">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="O10" s="8"/>
       <c r="P10" s="8"/>
       <c r="Q10" s="10">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="R10" s="8"/>
       <c r="S10" s="9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T10" s="8"/>
       <c r="U10" s="8"/>
       <c r="V10" s="8"/>
       <c r="W10" s="9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="X10" s="9">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="Y10" s="8"/>
       <c r="Z10" s="12"/>
       <c r="AA10" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AB10" s="8"/>
       <c r="AC10" s="8"/>
       <c r="AD10" s="8"/>
-      <c r="AE10" s="9">
-        <v>30</v>
+      <c r="AE10" s="10">
+        <v>20.5</v>
       </c>
       <c r="AF10" s="9">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="AG10" s="8"/>
       <c r="AH10" s="8"/>
@@ -1379,7 +1406,7 @@
         <v>68</v>
       </c>
       <c r="AK10" s="9">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AL10" s="7"/>
       <c r="AM10" s="7"/>
@@ -1388,44 +1415,76 @@
     </row>
     <row r="11" spans="1:41" ht="15.75" thickBot="1">
       <c r="A11" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
+      <c r="E11" s="9">
+        <v>2</v>
+      </c>
+      <c r="F11" s="9">
+        <v>2</v>
+      </c>
+      <c r="G11" s="9">
+        <v>2</v>
+      </c>
+      <c r="H11" s="9">
+        <v>2</v>
+      </c>
+      <c r="I11" s="9">
+        <v>2</v>
+      </c>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
+      <c r="M11" s="9">
+        <v>2</v>
+      </c>
+      <c r="N11" s="9">
+        <v>14</v>
+      </c>
       <c r="O11" s="8"/>
       <c r="P11" s="8"/>
-      <c r="Q11" s="8"/>
+      <c r="Q11" s="10">
+        <v>180</v>
+      </c>
       <c r="R11" s="8"/>
-      <c r="S11" s="8"/>
+      <c r="S11" s="9">
+        <v>2</v>
+      </c>
       <c r="T11" s="8"/>
       <c r="U11" s="8"/>
       <c r="V11" s="8"/>
-      <c r="W11" s="8"/>
-      <c r="X11" s="8"/>
+      <c r="W11" s="9">
+        <v>4</v>
+      </c>
+      <c r="X11" s="9">
+        <v>7</v>
+      </c>
       <c r="Y11" s="8"/>
       <c r="Z11" s="12"/>
-      <c r="AA11" s="8"/>
+      <c r="AA11" s="9">
+        <v>3</v>
+      </c>
       <c r="AB11" s="8"/>
       <c r="AC11" s="8"/>
       <c r="AD11" s="8"/>
-      <c r="AE11" s="8"/>
-      <c r="AF11" s="8"/>
+      <c r="AE11" s="9">
+        <v>30</v>
+      </c>
+      <c r="AF11" s="9">
+        <v>19</v>
+      </c>
       <c r="AG11" s="8"/>
       <c r="AH11" s="8"/>
       <c r="AI11" s="8"/>
-      <c r="AJ11" s="8"/>
-      <c r="AK11" s="8"/>
+      <c r="AJ11" s="10">
+        <v>68</v>
+      </c>
+      <c r="AK11" s="9">
+        <v>58</v>
+      </c>
       <c r="AL11" s="7"/>
       <c r="AM11" s="7"/>
       <c r="AN11" s="7"/>
@@ -1433,7 +1492,7 @@
     </row>
     <row r="12" spans="1:41" ht="15.75" thickBot="1">
       <c r="A12" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -1478,80 +1537,52 @@
     </row>
     <row r="13" spans="1:41" ht="15.75" thickBot="1">
       <c r="A13" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
-      <c r="E13" s="9">
-        <v>2</v>
-      </c>
-      <c r="F13" s="9">
-        <v>2</v>
-      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
-      <c r="M13" s="9">
-        <v>2</v>
-      </c>
-      <c r="N13" s="9">
-        <v>11</v>
-      </c>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
       <c r="O13" s="8"/>
       <c r="P13" s="8"/>
-      <c r="Q13" s="10">
-        <v>170</v>
-      </c>
+      <c r="Q13" s="8"/>
       <c r="R13" s="8"/>
-      <c r="S13" s="10">
-        <v>6</v>
-      </c>
+      <c r="S13" s="8"/>
       <c r="T13" s="8"/>
       <c r="U13" s="8"/>
-      <c r="V13" s="10">
-        <v>0</v>
-      </c>
-      <c r="W13" s="9">
-        <v>2</v>
-      </c>
-      <c r="X13" s="10">
-        <v>0</v>
-      </c>
+      <c r="V13" s="8"/>
+      <c r="W13" s="8"/>
+      <c r="X13" s="8"/>
       <c r="Y13" s="8"/>
       <c r="Z13" s="12"/>
-      <c r="AA13" s="9">
-        <v>3</v>
-      </c>
+      <c r="AA13" s="8"/>
       <c r="AB13" s="8"/>
       <c r="AC13" s="8"/>
       <c r="AD13" s="8"/>
-      <c r="AE13" s="10">
-        <v>40.75</v>
-      </c>
-      <c r="AF13" s="10">
-        <v>11</v>
-      </c>
+      <c r="AE13" s="8"/>
+      <c r="AF13" s="8"/>
       <c r="AG13" s="8"/>
       <c r="AH13" s="8"/>
       <c r="AI13" s="8"/>
-      <c r="AJ13" s="10">
-        <v>0</v>
-      </c>
+      <c r="AJ13" s="8"/>
       <c r="AK13" s="8"/>
-      <c r="AL13" s="9">
-        <v>32</v>
-      </c>
-      <c r="AM13" s="8"/>
+      <c r="AL13" s="7"/>
+      <c r="AM13" s="7"/>
       <c r="AN13" s="7"/>
       <c r="AO13" s="8"/>
     </row>
     <row r="14" spans="1:41" ht="15.75" thickBot="1">
       <c r="A14" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -1569,7 +1600,7 @@
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
       <c r="M14" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N14" s="9">
         <v>11</v>
@@ -1577,11 +1608,11 @@
       <c r="O14" s="8"/>
       <c r="P14" s="8"/>
       <c r="Q14" s="10">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="R14" s="8"/>
       <c r="S14" s="10">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T14" s="8"/>
       <c r="U14" s="8"/>
@@ -1589,79 +1620,107 @@
         <v>0</v>
       </c>
       <c r="W14" s="9">
-        <v>4</v>
-      </c>
-      <c r="X14" s="9">
+        <v>2</v>
+      </c>
+      <c r="X14" s="10">
         <v>0</v>
       </c>
       <c r="Y14" s="8"/>
       <c r="Z14" s="12"/>
       <c r="AA14" s="9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AB14" s="8"/>
       <c r="AC14" s="8"/>
       <c r="AD14" s="8"/>
-      <c r="AE14" s="9">
-        <v>17.5</v>
+      <c r="AE14" s="10">
+        <v>40.75</v>
       </c>
       <c r="AF14" s="10">
-        <v>41.5</v>
+        <v>11</v>
       </c>
       <c r="AG14" s="8"/>
       <c r="AH14" s="8"/>
       <c r="AI14" s="8"/>
       <c r="AJ14" s="10">
-        <v>58</v>
-      </c>
-      <c r="AK14" s="9">
-        <v>55.5</v>
-      </c>
-      <c r="AL14" s="8"/>
+        <v>0</v>
+      </c>
+      <c r="AK14" s="8"/>
+      <c r="AL14" s="9">
+        <v>32</v>
+      </c>
       <c r="AM14" s="8"/>
       <c r="AN14" s="7"/>
       <c r="AO14" s="8"/>
     </row>
     <row r="15" spans="1:41" ht="15.75" thickBot="1">
       <c r="A15" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
+      <c r="E15" s="9">
+        <v>2</v>
+      </c>
+      <c r="F15" s="9">
+        <v>2</v>
+      </c>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
       <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
+      <c r="M15" s="9">
+        <v>3</v>
+      </c>
+      <c r="N15" s="9">
+        <v>11</v>
+      </c>
       <c r="O15" s="8"/>
       <c r="P15" s="8"/>
-      <c r="Q15" s="8"/>
+      <c r="Q15" s="10">
+        <v>160</v>
+      </c>
       <c r="R15" s="8"/>
-      <c r="S15" s="8"/>
+      <c r="S15" s="10">
+        <v>5</v>
+      </c>
       <c r="T15" s="8"/>
       <c r="U15" s="8"/>
-      <c r="V15" s="8"/>
-      <c r="W15" s="8"/>
-      <c r="X15" s="8"/>
+      <c r="V15" s="10">
+        <v>0</v>
+      </c>
+      <c r="W15" s="9">
+        <v>4</v>
+      </c>
+      <c r="X15" s="9">
+        <v>0</v>
+      </c>
       <c r="Y15" s="8"/>
       <c r="Z15" s="12"/>
-      <c r="AA15" s="8"/>
+      <c r="AA15" s="9">
+        <v>5</v>
+      </c>
       <c r="AB15" s="8"/>
       <c r="AC15" s="8"/>
       <c r="AD15" s="8"/>
-      <c r="AE15" s="8"/>
-      <c r="AF15" s="8"/>
+      <c r="AE15" s="9">
+        <v>17.5</v>
+      </c>
+      <c r="AF15" s="10">
+        <v>41.5</v>
+      </c>
       <c r="AG15" s="8"/>
       <c r="AH15" s="8"/>
       <c r="AI15" s="8"/>
-      <c r="AJ15" s="8"/>
-      <c r="AK15" s="8"/>
+      <c r="AJ15" s="10">
+        <v>58</v>
+      </c>
+      <c r="AK15" s="9">
+        <v>55.5</v>
+      </c>
       <c r="AL15" s="8"/>
       <c r="AM15" s="8"/>
       <c r="AN15" s="7"/>
@@ -1669,78 +1728,44 @@
     </row>
     <row r="16" spans="1:41" ht="15.75" thickBot="1">
       <c r="A16" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
-      <c r="E16" s="9">
-        <v>2</v>
-      </c>
-      <c r="F16" s="9">
-        <v>2</v>
-      </c>
-      <c r="G16" s="9">
-        <v>2</v>
-      </c>
-      <c r="H16" s="9">
-        <v>2</v>
-      </c>
-      <c r="I16" s="9">
-        <v>2</v>
-      </c>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
       <c r="L16" s="8"/>
-      <c r="M16" s="10">
-        <v>3</v>
-      </c>
-      <c r="N16" s="9">
-        <v>14</v>
-      </c>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
       <c r="O16" s="8"/>
       <c r="P16" s="8"/>
-      <c r="Q16" s="10">
-        <v>180</v>
-      </c>
+      <c r="Q16" s="8"/>
       <c r="R16" s="8"/>
-      <c r="S16" s="9">
-        <v>5</v>
-      </c>
+      <c r="S16" s="8"/>
       <c r="T16" s="8"/>
       <c r="U16" s="8"/>
-      <c r="V16" s="10">
-        <v>0</v>
-      </c>
-      <c r="W16" s="9">
-        <v>3</v>
-      </c>
-      <c r="X16" s="10">
-        <v>3</v>
-      </c>
+      <c r="V16" s="8"/>
+      <c r="W16" s="8"/>
+      <c r="X16" s="8"/>
       <c r="Y16" s="8"/>
       <c r="Z16" s="12"/>
-      <c r="AA16" s="9">
-        <v>5</v>
-      </c>
+      <c r="AA16" s="8"/>
       <c r="AB16" s="8"/>
       <c r="AC16" s="8"/>
       <c r="AD16" s="8"/>
-      <c r="AE16" s="9">
-        <v>35</v>
-      </c>
-      <c r="AF16" s="9">
-        <v>42</v>
-      </c>
+      <c r="AE16" s="8"/>
+      <c r="AF16" s="8"/>
       <c r="AG16" s="8"/>
       <c r="AH16" s="8"/>
       <c r="AI16" s="8"/>
-      <c r="AJ16" s="10">
-        <v>72</v>
-      </c>
-      <c r="AK16" s="10">
-        <v>73</v>
-      </c>
+      <c r="AJ16" s="8"/>
+      <c r="AK16" s="8"/>
       <c r="AL16" s="8"/>
       <c r="AM16" s="8"/>
       <c r="AN16" s="7"/>
@@ -1748,44 +1773,78 @@
     </row>
     <row r="17" spans="1:41" ht="15.75" thickBot="1">
       <c r="A17" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
+      <c r="E17" s="9">
+        <v>2</v>
+      </c>
+      <c r="F17" s="9">
+        <v>2</v>
+      </c>
+      <c r="G17" s="9">
+        <v>2</v>
+      </c>
+      <c r="H17" s="9">
+        <v>2</v>
+      </c>
+      <c r="I17" s="9">
+        <v>2</v>
+      </c>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
+      <c r="M17" s="10">
+        <v>3</v>
+      </c>
+      <c r="N17" s="9">
+        <v>14</v>
+      </c>
       <c r="O17" s="8"/>
       <c r="P17" s="8"/>
-      <c r="Q17" s="8"/>
+      <c r="Q17" s="10">
+        <v>180</v>
+      </c>
       <c r="R17" s="8"/>
-      <c r="S17" s="8"/>
+      <c r="S17" s="9">
+        <v>5</v>
+      </c>
       <c r="T17" s="8"/>
       <c r="U17" s="8"/>
-      <c r="V17" s="8"/>
-      <c r="W17" s="8"/>
-      <c r="X17" s="8"/>
+      <c r="V17" s="10">
+        <v>0</v>
+      </c>
+      <c r="W17" s="9">
+        <v>3</v>
+      </c>
+      <c r="X17" s="10">
+        <v>3</v>
+      </c>
       <c r="Y17" s="8"/>
       <c r="Z17" s="12"/>
-      <c r="AA17" s="8"/>
+      <c r="AA17" s="9">
+        <v>5</v>
+      </c>
       <c r="AB17" s="8"/>
       <c r="AC17" s="8"/>
       <c r="AD17" s="8"/>
-      <c r="AE17" s="8"/>
-      <c r="AF17" s="8"/>
+      <c r="AE17" s="9">
+        <v>35</v>
+      </c>
+      <c r="AF17" s="9">
+        <v>42</v>
+      </c>
       <c r="AG17" s="8"/>
       <c r="AH17" s="8"/>
       <c r="AI17" s="8"/>
-      <c r="AJ17" s="8"/>
-      <c r="AK17" s="8"/>
+      <c r="AJ17" s="10">
+        <v>72</v>
+      </c>
+      <c r="AK17" s="10">
+        <v>73</v>
+      </c>
       <c r="AL17" s="8"/>
       <c r="AM17" s="8"/>
       <c r="AN17" s="7"/>
@@ -1793,70 +1852,44 @@
     </row>
     <row r="18" spans="1:41" ht="15.75" thickBot="1">
       <c r="A18" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
-      <c r="E18" s="9">
-        <v>2</v>
-      </c>
-      <c r="F18" s="9">
-        <v>2</v>
-      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
-      <c r="M18" s="9">
-        <v>7</v>
-      </c>
-      <c r="N18" s="9">
-        <v>11</v>
-      </c>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
-      <c r="Q18" s="10">
-        <v>60</v>
-      </c>
+      <c r="Q18" s="8"/>
       <c r="R18" s="8"/>
-      <c r="S18" s="10">
-        <v>5</v>
-      </c>
+      <c r="S18" s="8"/>
       <c r="T18" s="8"/>
       <c r="U18" s="8"/>
       <c r="V18" s="8"/>
-      <c r="W18" s="9">
-        <v>2</v>
-      </c>
-      <c r="X18" s="10">
-        <v>1</v>
-      </c>
+      <c r="W18" s="8"/>
+      <c r="X18" s="8"/>
       <c r="Y18" s="8"/>
       <c r="Z18" s="12"/>
-      <c r="AA18" s="9">
-        <v>5</v>
-      </c>
+      <c r="AA18" s="8"/>
       <c r="AB18" s="8"/>
       <c r="AC18" s="8"/>
       <c r="AD18" s="8"/>
-      <c r="AE18" s="10">
-        <v>79</v>
-      </c>
-      <c r="AF18" s="10">
-        <v>48</v>
-      </c>
+      <c r="AE18" s="8"/>
+      <c r="AF18" s="8"/>
       <c r="AG18" s="8"/>
       <c r="AH18" s="8"/>
       <c r="AI18" s="8"/>
-      <c r="AJ18" s="9">
-        <v>91</v>
-      </c>
-      <c r="AK18" s="9">
-        <v>80.5</v>
-      </c>
+      <c r="AJ18" s="8"/>
+      <c r="AK18" s="8"/>
       <c r="AL18" s="8"/>
       <c r="AM18" s="8"/>
       <c r="AN18" s="7"/>
@@ -1864,44 +1897,70 @@
     </row>
     <row r="19" spans="1:41" ht="15.75" thickBot="1">
       <c r="A19" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
+      <c r="E19" s="9">
+        <v>2</v>
+      </c>
+      <c r="F19" s="9">
+        <v>2</v>
+      </c>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
       <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
+      <c r="M19" s="9">
+        <v>7</v>
+      </c>
+      <c r="N19" s="9">
+        <v>11</v>
+      </c>
       <c r="O19" s="8"/>
       <c r="P19" s="8"/>
-      <c r="Q19" s="8"/>
+      <c r="Q19" s="10">
+        <v>60</v>
+      </c>
       <c r="R19" s="8"/>
-      <c r="S19" s="8"/>
+      <c r="S19" s="10">
+        <v>5</v>
+      </c>
       <c r="T19" s="8"/>
       <c r="U19" s="8"/>
       <c r="V19" s="8"/>
-      <c r="W19" s="8"/>
-      <c r="X19" s="8"/>
+      <c r="W19" s="9">
+        <v>2</v>
+      </c>
+      <c r="X19" s="10">
+        <v>1</v>
+      </c>
       <c r="Y19" s="8"/>
       <c r="Z19" s="12"/>
-      <c r="AA19" s="8"/>
+      <c r="AA19" s="9">
+        <v>5</v>
+      </c>
       <c r="AB19" s="8"/>
       <c r="AC19" s="8"/>
       <c r="AD19" s="8"/>
-      <c r="AE19" s="8"/>
-      <c r="AF19" s="8"/>
+      <c r="AE19" s="10">
+        <v>79</v>
+      </c>
+      <c r="AF19" s="10">
+        <v>48</v>
+      </c>
       <c r="AG19" s="8"/>
       <c r="AH19" s="8"/>
       <c r="AI19" s="8"/>
-      <c r="AJ19" s="8"/>
-      <c r="AK19" s="8"/>
+      <c r="AJ19" s="9">
+        <v>91</v>
+      </c>
+      <c r="AK19" s="9">
+        <v>80.5</v>
+      </c>
       <c r="AL19" s="8"/>
       <c r="AM19" s="8"/>
       <c r="AN19" s="7"/>
@@ -1909,7 +1968,7 @@
     </row>
     <row r="20" spans="1:41" ht="15.75" thickBot="1">
       <c r="A20" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -1945,12 +2004,8 @@
       <c r="AG20" s="8"/>
       <c r="AH20" s="8"/>
       <c r="AI20" s="8"/>
-      <c r="AJ20" s="10">
-        <v>0</v>
-      </c>
-      <c r="AK20" s="9">
-        <v>3</v>
-      </c>
+      <c r="AJ20" s="8"/>
+      <c r="AK20" s="8"/>
       <c r="AL20" s="8"/>
       <c r="AM20" s="8"/>
       <c r="AN20" s="7"/>
@@ -1958,75 +2013,47 @@
     </row>
     <row r="21" spans="1:41" ht="15.75" thickBot="1">
       <c r="A21" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
-      <c r="E21" s="9">
-        <v>2</v>
-      </c>
-      <c r="F21" s="9">
-        <v>2</v>
-      </c>
-      <c r="G21" s="9">
-        <v>2</v>
-      </c>
-      <c r="H21" s="9">
-        <v>2</v>
-      </c>
-      <c r="I21" s="9">
-        <v>2</v>
-      </c>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
-      <c r="M21" s="9">
-        <v>6</v>
-      </c>
-      <c r="N21" s="9">
-        <v>4</v>
-      </c>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
       <c r="O21" s="8"/>
       <c r="P21" s="8"/>
-      <c r="Q21" s="9">
-        <v>139</v>
-      </c>
+      <c r="Q21" s="8"/>
       <c r="R21" s="8"/>
-      <c r="S21" s="9">
-        <v>3</v>
-      </c>
+      <c r="S21" s="8"/>
       <c r="T21" s="8"/>
       <c r="U21" s="8"/>
       <c r="V21" s="8"/>
-      <c r="W21" s="9">
-        <v>4</v>
-      </c>
-      <c r="X21" s="10">
-        <v>12</v>
-      </c>
+      <c r="W21" s="8"/>
+      <c r="X21" s="8"/>
       <c r="Y21" s="8"/>
       <c r="Z21" s="12"/>
-      <c r="AA21" s="10">
-        <v>2</v>
-      </c>
+      <c r="AA21" s="8"/>
       <c r="AB21" s="8"/>
       <c r="AC21" s="8"/>
       <c r="AD21" s="8"/>
-      <c r="AE21" s="10">
-        <v>40</v>
-      </c>
-      <c r="AF21" s="9">
-        <v>32</v>
-      </c>
+      <c r="AE21" s="8"/>
+      <c r="AF21" s="8"/>
       <c r="AG21" s="8"/>
       <c r="AH21" s="8"/>
       <c r="AI21" s="8"/>
       <c r="AJ21" s="10">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="AK21" s="9">
-        <v>62</v>
+        <v>3</v>
       </c>
       <c r="AL21" s="8"/>
       <c r="AM21" s="8"/>
@@ -2035,7 +2062,7 @@
     </row>
     <row r="22" spans="1:41" ht="15.75" thickBot="1">
       <c r="A22" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -2058,108 +2085,140 @@
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
-      <c r="M22" s="10">
-        <v>5</v>
+      <c r="M22" s="9">
+        <v>6</v>
       </c>
       <c r="N22" s="9">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="O22" s="8"/>
       <c r="P22" s="8"/>
-      <c r="Q22" s="10">
-        <v>179</v>
+      <c r="Q22" s="9">
+        <v>139</v>
       </c>
       <c r="R22" s="8"/>
       <c r="S22" s="9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T22" s="8"/>
       <c r="U22" s="8"/>
       <c r="V22" s="8"/>
       <c r="W22" s="9">
-        <v>0</v>
-      </c>
-      <c r="X22" s="9">
-        <v>10</v>
+        <v>4</v>
+      </c>
+      <c r="X22" s="10">
+        <v>12</v>
       </c>
       <c r="Y22" s="8"/>
       <c r="Z22" s="12"/>
-      <c r="AA22" s="9">
+      <c r="AA22" s="10">
         <v>2</v>
       </c>
       <c r="AB22" s="8"/>
       <c r="AC22" s="8"/>
       <c r="AD22" s="8"/>
       <c r="AE22" s="10">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="AF22" s="9">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="AG22" s="8"/>
       <c r="AH22" s="8"/>
       <c r="AI22" s="8"/>
       <c r="AJ22" s="10">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="AK22" s="9">
-        <v>65.5</v>
+        <v>62</v>
       </c>
       <c r="AL22" s="8"/>
-      <c r="AM22" s="9">
-        <v>4</v>
-      </c>
+      <c r="AM22" s="8"/>
       <c r="AN22" s="7"/>
       <c r="AO22" s="8"/>
     </row>
     <row r="23" spans="1:41" ht="15.75" thickBot="1">
       <c r="A23" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
+      <c r="E23" s="9">
+        <v>2</v>
+      </c>
+      <c r="F23" s="9">
+        <v>2</v>
+      </c>
+      <c r="G23" s="9">
+        <v>2</v>
+      </c>
+      <c r="H23" s="9">
+        <v>2</v>
+      </c>
+      <c r="I23" s="9">
+        <v>2</v>
+      </c>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
-      <c r="N23" s="8"/>
+      <c r="M23" s="10">
+        <v>5</v>
+      </c>
+      <c r="N23" s="9">
+        <v>11</v>
+      </c>
       <c r="O23" s="8"/>
       <c r="P23" s="8"/>
-      <c r="Q23" s="8"/>
+      <c r="Q23" s="10">
+        <v>179</v>
+      </c>
       <c r="R23" s="8"/>
-      <c r="S23" s="8"/>
+      <c r="S23" s="9">
+        <v>1</v>
+      </c>
       <c r="T23" s="8"/>
       <c r="U23" s="8"/>
       <c r="V23" s="8"/>
-      <c r="W23" s="8"/>
-      <c r="X23" s="8"/>
+      <c r="W23" s="9">
+        <v>0</v>
+      </c>
+      <c r="X23" s="9">
+        <v>10</v>
+      </c>
       <c r="Y23" s="8"/>
       <c r="Z23" s="12"/>
-      <c r="AA23" s="8"/>
+      <c r="AA23" s="9">
+        <v>2</v>
+      </c>
       <c r="AB23" s="8"/>
       <c r="AC23" s="8"/>
       <c r="AD23" s="8"/>
-      <c r="AE23" s="8"/>
-      <c r="AF23" s="8"/>
+      <c r="AE23" s="10">
+        <v>33</v>
+      </c>
+      <c r="AF23" s="9">
+        <v>9</v>
+      </c>
       <c r="AG23" s="8"/>
       <c r="AH23" s="8"/>
       <c r="AI23" s="8"/>
-      <c r="AJ23" s="8"/>
-      <c r="AK23" s="8"/>
-      <c r="AL23" s="7"/>
-      <c r="AM23" s="7"/>
+      <c r="AJ23" s="10">
+        <v>67</v>
+      </c>
+      <c r="AK23" s="9">
+        <v>65.5</v>
+      </c>
+      <c r="AL23" s="8"/>
+      <c r="AM23" s="9">
+        <v>4</v>
+      </c>
       <c r="AN23" s="7"/>
       <c r="AO23" s="8"/>
     </row>
     <row r="24" spans="1:41" ht="15.75" thickBot="1">
       <c r="A24" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -2204,80 +2263,52 @@
     </row>
     <row r="25" spans="1:41" ht="15.75" thickBot="1">
       <c r="A25" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
-      <c r="E25" s="9">
-        <v>2</v>
-      </c>
-      <c r="F25" s="9">
-        <v>2</v>
-      </c>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
-      <c r="M25" s="10">
-        <v>5</v>
-      </c>
-      <c r="N25" s="9">
-        <v>11</v>
-      </c>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
       <c r="O25" s="8"/>
       <c r="P25" s="8"/>
-      <c r="Q25" s="10">
-        <v>160</v>
-      </c>
+      <c r="Q25" s="8"/>
       <c r="R25" s="8"/>
-      <c r="S25" s="10">
-        <v>4</v>
-      </c>
+      <c r="S25" s="8"/>
       <c r="T25" s="8"/>
       <c r="U25" s="8"/>
-      <c r="V25" s="10">
-        <v>0</v>
-      </c>
-      <c r="W25" s="9">
-        <v>5</v>
-      </c>
-      <c r="X25" s="9">
-        <v>23</v>
-      </c>
+      <c r="V25" s="8"/>
+      <c r="W25" s="8"/>
+      <c r="X25" s="8"/>
       <c r="Y25" s="8"/>
       <c r="Z25" s="12"/>
-      <c r="AA25" s="9">
-        <v>4</v>
-      </c>
+      <c r="AA25" s="8"/>
       <c r="AB25" s="8"/>
       <c r="AC25" s="8"/>
       <c r="AD25" s="8"/>
-      <c r="AE25" s="9">
-        <v>30.5</v>
-      </c>
-      <c r="AF25" s="10">
-        <v>53</v>
-      </c>
+      <c r="AE25" s="8"/>
+      <c r="AF25" s="8"/>
       <c r="AG25" s="8"/>
       <c r="AH25" s="8"/>
       <c r="AI25" s="8"/>
-      <c r="AJ25" s="9">
-        <v>91</v>
-      </c>
-      <c r="AK25" s="9">
-        <v>83.5</v>
-      </c>
-      <c r="AL25" s="8"/>
+      <c r="AJ25" s="8"/>
+      <c r="AK25" s="8"/>
+      <c r="AL25" s="7"/>
       <c r="AM25" s="7"/>
       <c r="AN25" s="7"/>
       <c r="AO25" s="8"/>
     </row>
     <row r="26" spans="1:41" ht="15.75" thickBot="1">
       <c r="A26" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -2294,8 +2325,8 @@
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
-      <c r="M26" s="9">
-        <v>1</v>
+      <c r="M26" s="10">
+        <v>5</v>
       </c>
       <c r="N26" s="9">
         <v>11</v>
@@ -2303,54 +2334,54 @@
       <c r="O26" s="8"/>
       <c r="P26" s="8"/>
       <c r="Q26" s="10">
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="R26" s="8"/>
-      <c r="S26" s="9">
-        <v>2</v>
+      <c r="S26" s="10">
+        <v>4</v>
       </c>
       <c r="T26" s="8"/>
       <c r="U26" s="8"/>
-      <c r="V26" s="8"/>
+      <c r="V26" s="10">
+        <v>0</v>
+      </c>
       <c r="W26" s="9">
         <v>5</v>
       </c>
       <c r="X26" s="9">
-        <v>15</v>
-      </c>
-      <c r="Y26" s="9">
-        <v>1</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="Y26" s="8"/>
       <c r="Z26" s="12"/>
       <c r="AA26" s="9">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AB26" s="8"/>
       <c r="AC26" s="8"/>
       <c r="AD26" s="8"/>
       <c r="AE26" s="9">
-        <v>13.5</v>
-      </c>
-      <c r="AF26" s="9">
-        <v>11</v>
+        <v>30.5</v>
+      </c>
+      <c r="AF26" s="10">
+        <v>53</v>
       </c>
       <c r="AG26" s="8"/>
       <c r="AH26" s="8"/>
       <c r="AI26" s="8"/>
-      <c r="AJ26" s="10">
-        <v>47</v>
+      <c r="AJ26" s="9">
+        <v>91</v>
       </c>
       <c r="AK26" s="9">
-        <v>41.5</v>
-      </c>
-      <c r="AL26" s="7"/>
+        <v>83.5</v>
+      </c>
+      <c r="AL26" s="8"/>
       <c r="AM26" s="7"/>
       <c r="AN26" s="7"/>
       <c r="AO26" s="8"/>
     </row>
     <row r="27" spans="1:41" ht="15.75" thickBot="1">
       <c r="A27" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
@@ -2361,68 +2392,60 @@
       <c r="F27" s="9">
         <v>2</v>
       </c>
-      <c r="G27" s="9">
-        <v>2</v>
-      </c>
-      <c r="H27" s="9">
-        <v>2</v>
-      </c>
-      <c r="I27" s="9">
-        <v>2</v>
-      </c>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
       <c r="J27" s="8"/>
       <c r="K27" s="8"/>
       <c r="L27" s="8"/>
       <c r="M27" s="9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N27" s="9">
         <v>11</v>
       </c>
       <c r="O27" s="8"/>
       <c r="P27" s="8"/>
-      <c r="Q27" s="9">
-        <v>171</v>
+      <c r="Q27" s="10">
+        <v>0</v>
       </c>
       <c r="R27" s="8"/>
       <c r="S27" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T27" s="8"/>
       <c r="U27" s="8"/>
-      <c r="V27" s="10">
-        <v>0</v>
-      </c>
+      <c r="V27" s="8"/>
       <c r="W27" s="9">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="X27" s="9">
-        <v>13</v>
-      </c>
-      <c r="Y27" s="10">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="Y27" s="9">
+        <v>1</v>
       </c>
       <c r="Z27" s="12"/>
       <c r="AA27" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB27" s="8"/>
       <c r="AC27" s="8"/>
       <c r="AD27" s="8"/>
-      <c r="AE27" s="10">
-        <v>38.5</v>
+      <c r="AE27" s="9">
+        <v>13.5</v>
       </c>
       <c r="AF27" s="9">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="AG27" s="8"/>
       <c r="AH27" s="8"/>
       <c r="AI27" s="8"/>
       <c r="AJ27" s="10">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="AK27" s="9">
-        <v>72.5</v>
+        <v>41.5</v>
       </c>
       <c r="AL27" s="7"/>
       <c r="AM27" s="7"/>
@@ -2431,44 +2454,80 @@
     </row>
     <row r="28" spans="1:41" ht="15.75" thickBot="1">
       <c r="A28" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
+      <c r="E28" s="9">
+        <v>2</v>
+      </c>
+      <c r="F28" s="9">
+        <v>2</v>
+      </c>
+      <c r="G28" s="9">
+        <v>2</v>
+      </c>
+      <c r="H28" s="9">
+        <v>2</v>
+      </c>
+      <c r="I28" s="9">
+        <v>2</v>
+      </c>
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
+      <c r="M28" s="9">
+        <v>4</v>
+      </c>
+      <c r="N28" s="9">
+        <v>11</v>
+      </c>
       <c r="O28" s="8"/>
       <c r="P28" s="8"/>
-      <c r="Q28" s="8"/>
+      <c r="Q28" s="9">
+        <v>171</v>
+      </c>
       <c r="R28" s="8"/>
-      <c r="S28" s="8"/>
+      <c r="S28" s="9">
+        <v>3</v>
+      </c>
       <c r="T28" s="8"/>
       <c r="U28" s="8"/>
-      <c r="V28" s="8"/>
-      <c r="W28" s="8"/>
-      <c r="X28" s="8"/>
-      <c r="Y28" s="8"/>
+      <c r="V28" s="10">
+        <v>0</v>
+      </c>
+      <c r="W28" s="9">
+        <v>2</v>
+      </c>
+      <c r="X28" s="9">
+        <v>13</v>
+      </c>
+      <c r="Y28" s="10">
+        <v>0</v>
+      </c>
       <c r="Z28" s="12"/>
-      <c r="AA28" s="8"/>
+      <c r="AA28" s="9">
+        <v>2</v>
+      </c>
       <c r="AB28" s="8"/>
       <c r="AC28" s="8"/>
       <c r="AD28" s="8"/>
-      <c r="AE28" s="8"/>
-      <c r="AF28" s="8"/>
+      <c r="AE28" s="10">
+        <v>38.5</v>
+      </c>
+      <c r="AF28" s="9">
+        <v>29</v>
+      </c>
       <c r="AG28" s="8"/>
       <c r="AH28" s="8"/>
       <c r="AI28" s="8"/>
-      <c r="AJ28" s="8"/>
-      <c r="AK28" s="8"/>
+      <c r="AJ28" s="10">
+        <v>78</v>
+      </c>
+      <c r="AK28" s="9">
+        <v>72.5</v>
+      </c>
       <c r="AL28" s="7"/>
       <c r="AM28" s="7"/>
       <c r="AN28" s="7"/>
@@ -2476,70 +2535,44 @@
     </row>
     <row r="29" spans="1:41" ht="15.75" thickBot="1">
       <c r="A29" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
-      <c r="E29" s="9">
-        <v>2</v>
-      </c>
-      <c r="F29" s="9">
-        <v>2</v>
-      </c>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
       <c r="K29" s="8"/>
       <c r="L29" s="8"/>
-      <c r="M29" s="9">
-        <v>4</v>
-      </c>
-      <c r="N29" s="9">
-        <v>9</v>
-      </c>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
       <c r="O29" s="8"/>
       <c r="P29" s="8"/>
-      <c r="Q29" s="10">
-        <v>162</v>
-      </c>
+      <c r="Q29" s="8"/>
       <c r="R29" s="8"/>
-      <c r="S29" s="9">
-        <v>5</v>
-      </c>
+      <c r="S29" s="8"/>
       <c r="T29" s="8"/>
       <c r="U29" s="8"/>
       <c r="V29" s="8"/>
-      <c r="W29" s="9">
-        <v>7</v>
-      </c>
-      <c r="X29" s="10">
-        <v>20</v>
-      </c>
+      <c r="W29" s="8"/>
+      <c r="X29" s="8"/>
       <c r="Y29" s="8"/>
       <c r="Z29" s="12"/>
-      <c r="AA29" s="9">
-        <v>2</v>
-      </c>
+      <c r="AA29" s="8"/>
       <c r="AB29" s="8"/>
       <c r="AC29" s="8"/>
       <c r="AD29" s="8"/>
-      <c r="AE29" s="10">
-        <v>40</v>
-      </c>
-      <c r="AF29" s="9">
-        <v>35</v>
-      </c>
+      <c r="AE29" s="8"/>
+      <c r="AF29" s="8"/>
       <c r="AG29" s="8"/>
       <c r="AH29" s="8"/>
       <c r="AI29" s="8"/>
-      <c r="AJ29" s="9">
-        <v>91</v>
-      </c>
-      <c r="AK29" s="9">
-        <v>87.5</v>
-      </c>
+      <c r="AJ29" s="8"/>
+      <c r="AK29" s="8"/>
       <c r="AL29" s="7"/>
       <c r="AM29" s="7"/>
       <c r="AN29" s="7"/>
@@ -2547,46 +2580,70 @@
     </row>
     <row r="30" spans="1:41" ht="15.75" thickBot="1">
       <c r="A30" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
+      <c r="E30" s="9">
+        <v>2</v>
+      </c>
+      <c r="F30" s="9">
+        <v>2</v>
+      </c>
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
       <c r="K30" s="8"/>
       <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
-      <c r="N30" s="8"/>
+      <c r="M30" s="9">
+        <v>4</v>
+      </c>
+      <c r="N30" s="9">
+        <v>9</v>
+      </c>
       <c r="O30" s="8"/>
       <c r="P30" s="8"/>
       <c r="Q30" s="10">
-        <v>0</v>
+        <v>162</v>
       </c>
       <c r="R30" s="8"/>
-      <c r="S30" s="8"/>
+      <c r="S30" s="9">
+        <v>5</v>
+      </c>
       <c r="T30" s="8"/>
       <c r="U30" s="8"/>
       <c r="V30" s="8"/>
-      <c r="W30" s="8"/>
-      <c r="X30" s="8"/>
+      <c r="W30" s="9">
+        <v>7</v>
+      </c>
+      <c r="X30" s="10">
+        <v>20</v>
+      </c>
       <c r="Y30" s="8"/>
       <c r="Z30" s="12"/>
-      <c r="AA30" s="8"/>
+      <c r="AA30" s="9">
+        <v>2</v>
+      </c>
       <c r="AB30" s="8"/>
       <c r="AC30" s="8"/>
       <c r="AD30" s="8"/>
-      <c r="AE30" s="8"/>
-      <c r="AF30" s="8"/>
+      <c r="AE30" s="10">
+        <v>40</v>
+      </c>
+      <c r="AF30" s="9">
+        <v>35</v>
+      </c>
       <c r="AG30" s="8"/>
       <c r="AH30" s="8"/>
       <c r="AI30" s="8"/>
-      <c r="AJ30" s="8"/>
-      <c r="AK30" s="8"/>
+      <c r="AJ30" s="9">
+        <v>91</v>
+      </c>
+      <c r="AK30" s="9">
+        <v>87.5</v>
+      </c>
       <c r="AL30" s="7"/>
       <c r="AM30" s="7"/>
       <c r="AN30" s="7"/>
@@ -2594,7 +2651,7 @@
     </row>
     <row r="31" spans="1:41" ht="15.75" thickBot="1">
       <c r="A31" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
@@ -2611,7 +2668,9 @@
       <c r="N31" s="8"/>
       <c r="O31" s="8"/>
       <c r="P31" s="8"/>
-      <c r="Q31" s="8"/>
+      <c r="Q31" s="10">
+        <v>0</v>
+      </c>
       <c r="R31" s="8"/>
       <c r="S31" s="8"/>
       <c r="T31" s="8"/>
@@ -2632,89 +2691,59 @@
       <c r="AI31" s="8"/>
       <c r="AJ31" s="8"/>
       <c r="AK31" s="8"/>
-      <c r="AL31" s="8"/>
+      <c r="AL31" s="7"/>
       <c r="AM31" s="7"/>
       <c r="AN31" s="7"/>
       <c r="AO31" s="8"/>
     </row>
     <row r="32" spans="1:41" ht="15.75" thickBot="1">
       <c r="A32" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
-      <c r="E32" s="9">
-        <v>2</v>
-      </c>
-      <c r="F32" s="9">
-        <v>2</v>
-      </c>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
       <c r="I32" s="8"/>
       <c r="J32" s="8"/>
       <c r="K32" s="8"/>
       <c r="L32" s="8"/>
-      <c r="M32" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="N32" s="9">
-        <v>19</v>
-      </c>
+      <c r="M32" s="8"/>
+      <c r="N32" s="8"/>
       <c r="O32" s="8"/>
-      <c r="P32" s="9">
-        <v>42</v>
-      </c>
-      <c r="Q32" s="9">
-        <v>52</v>
-      </c>
+      <c r="P32" s="8"/>
+      <c r="Q32" s="8"/>
       <c r="R32" s="8"/>
-      <c r="S32" s="9">
-        <v>4</v>
-      </c>
+      <c r="S32" s="8"/>
       <c r="T32" s="8"/>
       <c r="U32" s="8"/>
       <c r="V32" s="8"/>
-      <c r="W32" s="9">
-        <v>4</v>
-      </c>
-      <c r="X32" s="9">
-        <v>23</v>
-      </c>
+      <c r="W32" s="8"/>
+      <c r="X32" s="8"/>
       <c r="Y32" s="8"/>
       <c r="Z32" s="12"/>
-      <c r="AA32" s="9">
-        <v>2</v>
-      </c>
+      <c r="AA32" s="8"/>
       <c r="AB32" s="8"/>
       <c r="AC32" s="8"/>
       <c r="AD32" s="8"/>
-      <c r="AE32" s="9">
-        <v>54.5</v>
-      </c>
-      <c r="AF32" s="9">
-        <v>40</v>
-      </c>
+      <c r="AE32" s="8"/>
+      <c r="AF32" s="8"/>
       <c r="AG32" s="8"/>
       <c r="AH32" s="8"/>
       <c r="AI32" s="8"/>
-      <c r="AJ32" s="9">
-        <v>91</v>
-      </c>
-      <c r="AK32" s="9">
-        <v>75.5</v>
-      </c>
-      <c r="AL32" s="7"/>
-      <c r="AM32" s="9">
-        <v>2</v>
-      </c>
+      <c r="AJ32" s="8"/>
+      <c r="AK32" s="8"/>
+      <c r="AL32" s="8"/>
+      <c r="AM32" s="7"/>
       <c r="AN32" s="7"/>
       <c r="AO32" s="8"/>
     </row>
     <row r="33" spans="1:41" ht="15.75" thickBot="1">
       <c r="A33" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
@@ -2732,44 +2761,44 @@
       <c r="K33" s="8"/>
       <c r="L33" s="8"/>
       <c r="M33" s="9">
-        <v>10</v>
+        <v>2.5</v>
       </c>
       <c r="N33" s="9">
         <v>19</v>
       </c>
       <c r="O33" s="8"/>
       <c r="P33" s="9">
-        <v>36</v>
-      </c>
-      <c r="Q33" s="8"/>
+        <v>42</v>
+      </c>
+      <c r="Q33" s="9">
+        <v>52</v>
+      </c>
       <c r="R33" s="8"/>
       <c r="S33" s="9">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="T33" s="8"/>
       <c r="U33" s="8"/>
-      <c r="V33" s="10">
-        <v>0</v>
-      </c>
+      <c r="V33" s="8"/>
       <c r="W33" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="X33" s="9">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="Y33" s="8"/>
       <c r="Z33" s="12"/>
       <c r="AA33" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AB33" s="8"/>
       <c r="AC33" s="8"/>
       <c r="AD33" s="8"/>
       <c r="AE33" s="9">
-        <v>65</v>
-      </c>
-      <c r="AF33" s="10">
-        <v>71</v>
+        <v>54.5</v>
+      </c>
+      <c r="AF33" s="9">
+        <v>40</v>
       </c>
       <c r="AG33" s="8"/>
       <c r="AH33" s="8"/>
@@ -2778,16 +2807,18 @@
         <v>91</v>
       </c>
       <c r="AK33" s="9">
-        <v>81</v>
+        <v>75.5</v>
       </c>
       <c r="AL33" s="7"/>
-      <c r="AM33" s="7"/>
+      <c r="AM33" s="9">
+        <v>2</v>
+      </c>
       <c r="AN33" s="7"/>
       <c r="AO33" s="8"/>
     </row>
     <row r="34" spans="1:41" ht="15.75" thickBot="1">
       <c r="A34" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
@@ -2805,21 +2836,19 @@
       <c r="K34" s="8"/>
       <c r="L34" s="8"/>
       <c r="M34" s="9">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="N34" s="9">
         <v>19</v>
       </c>
       <c r="O34" s="8"/>
-      <c r="P34" s="10">
-        <v>38</v>
-      </c>
-      <c r="Q34" s="9">
-        <v>120</v>
-      </c>
+      <c r="P34" s="9">
+        <v>36</v>
+      </c>
+      <c r="Q34" s="8"/>
       <c r="R34" s="8"/>
       <c r="S34" s="9">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="T34" s="8"/>
       <c r="U34" s="8"/>
@@ -2827,24 +2856,24 @@
         <v>0</v>
       </c>
       <c r="W34" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="X34" s="9">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="Y34" s="8"/>
       <c r="Z34" s="12"/>
       <c r="AA34" s="9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AB34" s="8"/>
       <c r="AC34" s="8"/>
       <c r="AD34" s="8"/>
-      <c r="AE34" s="10">
-        <v>72.5</v>
-      </c>
-      <c r="AF34" s="9">
-        <v>61</v>
+      <c r="AE34" s="9">
+        <v>65</v>
+      </c>
+      <c r="AF34" s="10">
+        <v>71</v>
       </c>
       <c r="AG34" s="8"/>
       <c r="AH34" s="8"/>
@@ -2853,7 +2882,7 @@
         <v>91</v>
       </c>
       <c r="AK34" s="9">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="AL34" s="7"/>
       <c r="AM34" s="7"/>
@@ -2862,44 +2891,74 @@
     </row>
     <row r="35" spans="1:41" ht="15.75" thickBot="1">
       <c r="A35" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
+      <c r="E35" s="9">
+        <v>2</v>
+      </c>
+      <c r="F35" s="9">
+        <v>2</v>
+      </c>
       <c r="G35" s="8"/>
       <c r="H35" s="8"/>
       <c r="I35" s="8"/>
       <c r="J35" s="8"/>
       <c r="K35" s="8"/>
       <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
-      <c r="N35" s="8"/>
+      <c r="M35" s="9">
+        <v>7</v>
+      </c>
+      <c r="N35" s="9">
+        <v>19</v>
+      </c>
       <c r="O35" s="8"/>
-      <c r="P35" s="8"/>
-      <c r="Q35" s="8"/>
+      <c r="P35" s="10">
+        <v>38</v>
+      </c>
+      <c r="Q35" s="9">
+        <v>120</v>
+      </c>
       <c r="R35" s="8"/>
-      <c r="S35" s="8"/>
+      <c r="S35" s="9">
+        <v>2</v>
+      </c>
       <c r="T35" s="8"/>
       <c r="U35" s="8"/>
-      <c r="V35" s="8"/>
-      <c r="W35" s="8"/>
-      <c r="X35" s="8"/>
+      <c r="V35" s="10">
+        <v>0</v>
+      </c>
+      <c r="W35" s="9">
+        <v>2</v>
+      </c>
+      <c r="X35" s="9">
+        <v>21</v>
+      </c>
       <c r="Y35" s="8"/>
       <c r="Z35" s="12"/>
-      <c r="AA35" s="8"/>
+      <c r="AA35" s="9">
+        <v>5</v>
+      </c>
       <c r="AB35" s="8"/>
       <c r="AC35" s="8"/>
       <c r="AD35" s="8"/>
-      <c r="AE35" s="8"/>
-      <c r="AF35" s="8"/>
+      <c r="AE35" s="10">
+        <v>72.5</v>
+      </c>
+      <c r="AF35" s="9">
+        <v>61</v>
+      </c>
       <c r="AG35" s="8"/>
       <c r="AH35" s="8"/>
       <c r="AI35" s="8"/>
-      <c r="AJ35" s="8"/>
-      <c r="AK35" s="8"/>
+      <c r="AJ35" s="9">
+        <v>91</v>
+      </c>
+      <c r="AK35" s="9">
+        <v>91</v>
+      </c>
       <c r="AL35" s="7"/>
       <c r="AM35" s="7"/>
       <c r="AN35" s="7"/>
@@ -2907,84 +2966,52 @@
     </row>
     <row r="36" spans="1:41" ht="15.75" thickBot="1">
       <c r="A36" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
-      <c r="E36" s="9">
-        <v>2</v>
-      </c>
-      <c r="F36" s="9">
-        <v>2</v>
-      </c>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
       <c r="G36" s="8"/>
       <c r="H36" s="8"/>
       <c r="I36" s="8"/>
       <c r="J36" s="8"/>
       <c r="K36" s="8"/>
       <c r="L36" s="8"/>
-      <c r="M36" s="9">
-        <v>11</v>
-      </c>
-      <c r="N36" s="9">
-        <v>19</v>
-      </c>
+      <c r="M36" s="8"/>
+      <c r="N36" s="8"/>
       <c r="O36" s="8"/>
-      <c r="P36" s="10">
-        <v>38</v>
-      </c>
-      <c r="Q36" s="9">
-        <v>56</v>
-      </c>
+      <c r="P36" s="8"/>
+      <c r="Q36" s="8"/>
       <c r="R36" s="8"/>
-      <c r="S36" s="9">
-        <v>4</v>
-      </c>
+      <c r="S36" s="8"/>
       <c r="T36" s="8"/>
       <c r="U36" s="8"/>
       <c r="V36" s="8"/>
-      <c r="W36" s="9">
-        <v>5</v>
-      </c>
-      <c r="X36" s="9">
-        <v>21</v>
-      </c>
+      <c r="W36" s="8"/>
+      <c r="X36" s="8"/>
       <c r="Y36" s="8"/>
       <c r="Z36" s="12"/>
-      <c r="AA36" s="9">
-        <v>4</v>
-      </c>
+      <c r="AA36" s="8"/>
       <c r="AB36" s="8"/>
       <c r="AC36" s="8"/>
       <c r="AD36" s="8"/>
-      <c r="AE36" s="10">
-        <v>73.5</v>
-      </c>
-      <c r="AF36" s="9">
-        <v>51</v>
-      </c>
-      <c r="AG36" s="9">
-        <v>0</v>
-      </c>
+      <c r="AE36" s="8"/>
+      <c r="AF36" s="8"/>
+      <c r="AG36" s="8"/>
       <c r="AH36" s="8"/>
       <c r="AI36" s="8"/>
-      <c r="AJ36" s="9">
-        <v>91</v>
-      </c>
-      <c r="AK36" s="9">
-        <v>89.5</v>
-      </c>
+      <c r="AJ36" s="8"/>
+      <c r="AK36" s="8"/>
       <c r="AL36" s="7"/>
-      <c r="AM36" s="9">
-        <v>4</v>
-      </c>
+      <c r="AM36" s="7"/>
       <c r="AN36" s="7"/>
       <c r="AO36" s="8"/>
     </row>
     <row r="37" spans="1:41" ht="15.75" thickBot="1">
       <c r="A37" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
@@ -3002,7 +3029,7 @@
       <c r="K37" s="8"/>
       <c r="L37" s="8"/>
       <c r="M37" s="9">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N37" s="9">
         <v>19</v>
@@ -3011,97 +3038,89 @@
       <c r="P37" s="10">
         <v>38</v>
       </c>
-      <c r="Q37" s="10">
-        <v>180</v>
+      <c r="Q37" s="9">
+        <v>56</v>
       </c>
       <c r="R37" s="8"/>
       <c r="S37" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T37" s="8"/>
       <c r="U37" s="8"/>
-      <c r="V37" s="10">
-        <v>0</v>
-      </c>
+      <c r="V37" s="8"/>
       <c r="W37" s="9">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="X37" s="9">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="Y37" s="8"/>
       <c r="Z37" s="12"/>
       <c r="AA37" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AB37" s="8"/>
       <c r="AC37" s="8"/>
       <c r="AD37" s="8"/>
       <c r="AE37" s="10">
-        <v>41</v>
-      </c>
-      <c r="AF37" s="10">
-        <v>46</v>
-      </c>
-      <c r="AG37" s="10">
+        <v>73.5</v>
+      </c>
+      <c r="AF37" s="9">
+        <v>51</v>
+      </c>
+      <c r="AG37" s="9">
         <v>0</v>
       </c>
-      <c r="AH37" s="9">
-        <v>0.5</v>
-      </c>
+      <c r="AH37" s="8"/>
       <c r="AI37" s="8"/>
       <c r="AJ37" s="9">
         <v>91</v>
       </c>
       <c r="AK37" s="9">
-        <v>85</v>
+        <v>89.5</v>
       </c>
       <c r="AL37" s="7"/>
-      <c r="AM37" s="8"/>
+      <c r="AM37" s="9">
+        <v>4</v>
+      </c>
       <c r="AN37" s="7"/>
       <c r="AO37" s="8"/>
     </row>
     <row r="38" spans="1:41" ht="15.75" thickBot="1">
       <c r="A38" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38" s="9">
-        <v>2</v>
-      </c>
-      <c r="C38" s="9">
-        <v>3</v>
-      </c>
-      <c r="D38" s="9">
-        <v>3</v>
-      </c>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
+        <v>36</v>
+      </c>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="9">
+        <v>2</v>
+      </c>
+      <c r="F38" s="9">
+        <v>2</v>
+      </c>
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
       <c r="I38" s="8"/>
-      <c r="J38" s="9">
-        <v>2</v>
-      </c>
-      <c r="K38" s="9">
-        <v>1</v>
-      </c>
-      <c r="L38" s="9">
-        <v>2</v>
-      </c>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
+      <c r="L38" s="8"/>
       <c r="M38" s="9">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="N38" s="9">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="O38" s="8"/>
-      <c r="P38" s="8"/>
-      <c r="Q38" s="9">
-        <v>24</v>
+      <c r="P38" s="10">
+        <v>38</v>
+      </c>
+      <c r="Q38" s="10">
+        <v>180</v>
       </c>
       <c r="R38" s="8"/>
       <c r="S38" s="9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="T38" s="8"/>
       <c r="U38" s="8"/>
@@ -3109,44 +3128,46 @@
         <v>0</v>
       </c>
       <c r="W38" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="X38" s="9">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="Y38" s="8"/>
       <c r="Z38" s="12"/>
       <c r="AA38" s="9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AB38" s="8"/>
       <c r="AC38" s="8"/>
       <c r="AD38" s="8"/>
       <c r="AE38" s="10">
-        <v>87</v>
-      </c>
-      <c r="AF38" s="9">
-        <v>58</v>
-      </c>
-      <c r="AG38" s="8"/>
-      <c r="AH38" s="8"/>
+        <v>41</v>
+      </c>
+      <c r="AF38" s="10">
+        <v>46</v>
+      </c>
+      <c r="AG38" s="10">
+        <v>0</v>
+      </c>
+      <c r="AH38" s="9">
+        <v>0.5</v>
+      </c>
       <c r="AI38" s="8"/>
-      <c r="AJ38" s="10">
-        <v>66</v>
+      <c r="AJ38" s="9">
+        <v>91</v>
       </c>
       <c r="AK38" s="9">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="AL38" s="7"/>
-      <c r="AM38" s="9">
-        <v>1</v>
-      </c>
+      <c r="AM38" s="8"/>
       <c r="AN38" s="7"/>
       <c r="AO38" s="8"/>
     </row>
     <row r="39" spans="1:41" ht="15.75" thickBot="1">
       <c r="A39" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" s="9">
         <v>2</v>
@@ -3163,49 +3184,73 @@
       <c r="H39" s="8"/>
       <c r="I39" s="8"/>
       <c r="J39" s="9">
+        <v>2</v>
+      </c>
+      <c r="K39" s="9">
         <v>1</v>
       </c>
-      <c r="K39" s="8"/>
       <c r="L39" s="9">
-        <v>1</v>
-      </c>
-      <c r="M39" s="8"/>
-      <c r="N39" s="8"/>
+        <v>2</v>
+      </c>
+      <c r="M39" s="9">
+        <v>5</v>
+      </c>
+      <c r="N39" s="9">
+        <v>10</v>
+      </c>
       <c r="O39" s="8"/>
       <c r="P39" s="8"/>
-      <c r="Q39" s="8"/>
+      <c r="Q39" s="9">
+        <v>24</v>
+      </c>
       <c r="R39" s="8"/>
-      <c r="S39" s="8"/>
+      <c r="S39" s="9">
+        <v>4</v>
+      </c>
       <c r="T39" s="8"/>
       <c r="U39" s="8"/>
-      <c r="V39" s="8"/>
-      <c r="W39" s="8"/>
-      <c r="X39" s="8"/>
+      <c r="V39" s="10">
+        <v>0</v>
+      </c>
+      <c r="W39" s="9">
+        <v>3</v>
+      </c>
+      <c r="X39" s="9">
+        <v>15</v>
+      </c>
       <c r="Y39" s="8"/>
       <c r="Z39" s="12"/>
-      <c r="AA39" s="8"/>
+      <c r="AA39" s="9">
+        <v>1</v>
+      </c>
       <c r="AB39" s="8"/>
       <c r="AC39" s="8"/>
       <c r="AD39" s="8"/>
-      <c r="AE39" s="8"/>
-      <c r="AF39" s="8"/>
+      <c r="AE39" s="10">
+        <v>87</v>
+      </c>
+      <c r="AF39" s="9">
+        <v>58</v>
+      </c>
       <c r="AG39" s="8"/>
       <c r="AH39" s="8"/>
       <c r="AI39" s="8"/>
       <c r="AJ39" s="10">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="AK39" s="9">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="AL39" s="7"/>
-      <c r="AM39" s="7"/>
+      <c r="AM39" s="9">
+        <v>1</v>
+      </c>
       <c r="AN39" s="7"/>
       <c r="AO39" s="8"/>
     </row>
     <row r="40" spans="1:41" ht="15.75" thickBot="1">
       <c r="A40" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" s="9">
         <v>2</v>
@@ -3222,56 +3267,40 @@
       <c r="H40" s="8"/>
       <c r="I40" s="8"/>
       <c r="J40" s="9">
-        <v>2</v>
-      </c>
-      <c r="K40" s="9">
         <v>1</v>
       </c>
+      <c r="K40" s="8"/>
       <c r="L40" s="9">
-        <v>2</v>
-      </c>
-      <c r="M40" s="9">
-        <v>2</v>
-      </c>
-      <c r="N40" s="9">
-        <v>10</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="M40" s="8"/>
+      <c r="N40" s="8"/>
       <c r="O40" s="8"/>
       <c r="P40" s="8"/>
       <c r="Q40" s="8"/>
       <c r="R40" s="8"/>
-      <c r="S40" s="9">
-        <v>1</v>
-      </c>
+      <c r="S40" s="8"/>
       <c r="T40" s="8"/>
       <c r="U40" s="8"/>
       <c r="V40" s="8"/>
-      <c r="W40" s="9">
-        <v>1</v>
-      </c>
-      <c r="X40" s="9">
-        <v>10</v>
-      </c>
+      <c r="W40" s="8"/>
+      <c r="X40" s="8"/>
       <c r="Y40" s="8"/>
       <c r="Z40" s="12"/>
       <c r="AA40" s="8"/>
       <c r="AB40" s="8"/>
       <c r="AC40" s="8"/>
       <c r="AD40" s="8"/>
-      <c r="AE40" s="10">
-        <v>15.75</v>
-      </c>
-      <c r="AF40" s="9">
-        <v>13</v>
-      </c>
+      <c r="AE40" s="8"/>
+      <c r="AF40" s="8"/>
       <c r="AG40" s="8"/>
       <c r="AH40" s="8"/>
       <c r="AI40" s="8"/>
       <c r="AJ40" s="10">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="AK40" s="9">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="AL40" s="7"/>
       <c r="AM40" s="7"/>
@@ -3280,7 +3309,7 @@
     </row>
     <row r="41" spans="1:41" ht="15.75" thickBot="1">
       <c r="A41" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41" s="9">
         <v>2</v>
@@ -3297,40 +3326,56 @@
       <c r="H41" s="8"/>
       <c r="I41" s="8"/>
       <c r="J41" s="9">
+        <v>2</v>
+      </c>
+      <c r="K41" s="9">
         <v>1</v>
       </c>
-      <c r="K41" s="8"/>
       <c r="L41" s="9">
-        <v>1</v>
-      </c>
-      <c r="M41" s="8"/>
-      <c r="N41" s="8"/>
+        <v>2</v>
+      </c>
+      <c r="M41" s="9">
+        <v>2</v>
+      </c>
+      <c r="N41" s="9">
+        <v>10</v>
+      </c>
       <c r="O41" s="8"/>
       <c r="P41" s="8"/>
       <c r="Q41" s="8"/>
       <c r="R41" s="8"/>
-      <c r="S41" s="8"/>
+      <c r="S41" s="9">
+        <v>1</v>
+      </c>
       <c r="T41" s="8"/>
       <c r="U41" s="8"/>
       <c r="V41" s="8"/>
-      <c r="W41" s="8"/>
-      <c r="X41" s="8"/>
+      <c r="W41" s="9">
+        <v>1</v>
+      </c>
+      <c r="X41" s="9">
+        <v>10</v>
+      </c>
       <c r="Y41" s="8"/>
       <c r="Z41" s="12"/>
       <c r="AA41" s="8"/>
       <c r="AB41" s="8"/>
       <c r="AC41" s="8"/>
       <c r="AD41" s="8"/>
-      <c r="AE41" s="8"/>
-      <c r="AF41" s="8"/>
+      <c r="AE41" s="10">
+        <v>15.75</v>
+      </c>
+      <c r="AF41" s="9">
+        <v>13</v>
+      </c>
       <c r="AG41" s="8"/>
       <c r="AH41" s="8"/>
       <c r="AI41" s="8"/>
       <c r="AJ41" s="10">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="AK41" s="9">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="AL41" s="7"/>
       <c r="AM41" s="7"/>
@@ -3339,7 +3384,7 @@
     </row>
     <row r="42" spans="1:41" ht="15.75" thickBot="1">
       <c r="A42" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" s="9">
         <v>2</v>
@@ -3386,7 +3431,7 @@
       <c r="AH42" s="8"/>
       <c r="AI42" s="8"/>
       <c r="AJ42" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK42" s="9">
         <v>3</v>
@@ -3398,7 +3443,7 @@
     </row>
     <row r="43" spans="1:41" ht="15.75" thickBot="1">
       <c r="A43" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43" s="9">
         <v>2</v>
@@ -3415,62 +3460,40 @@
       <c r="H43" s="8"/>
       <c r="I43" s="8"/>
       <c r="J43" s="9">
-        <v>2</v>
-      </c>
-      <c r="K43" s="9">
         <v>1</v>
       </c>
+      <c r="K43" s="8"/>
       <c r="L43" s="9">
-        <v>2</v>
-      </c>
-      <c r="M43" s="9">
-        <v>8</v>
-      </c>
-      <c r="N43" s="9">
-        <v>15</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="M43" s="8"/>
+      <c r="N43" s="8"/>
       <c r="O43" s="8"/>
       <c r="P43" s="8"/>
-      <c r="Q43" s="9">
-        <v>63</v>
-      </c>
+      <c r="Q43" s="8"/>
       <c r="R43" s="8"/>
-      <c r="S43" s="9">
-        <v>3</v>
-      </c>
+      <c r="S43" s="8"/>
       <c r="T43" s="8"/>
       <c r="U43" s="8"/>
-      <c r="V43" s="10">
-        <v>0</v>
-      </c>
-      <c r="W43" s="9">
-        <v>2</v>
-      </c>
-      <c r="X43" s="9">
-        <v>10</v>
-      </c>
+      <c r="V43" s="8"/>
+      <c r="W43" s="8"/>
+      <c r="X43" s="8"/>
       <c r="Y43" s="8"/>
       <c r="Z43" s="12"/>
-      <c r="AA43" s="9">
-        <v>3</v>
-      </c>
+      <c r="AA43" s="8"/>
       <c r="AB43" s="8"/>
       <c r="AC43" s="8"/>
       <c r="AD43" s="8"/>
-      <c r="AE43" s="9">
-        <v>104</v>
-      </c>
-      <c r="AF43" s="9">
-        <v>62</v>
-      </c>
+      <c r="AE43" s="8"/>
+      <c r="AF43" s="8"/>
       <c r="AG43" s="8"/>
       <c r="AH43" s="8"/>
       <c r="AI43" s="8"/>
-      <c r="AJ43" s="9">
-        <v>82</v>
+      <c r="AJ43" s="10">
+        <v>0</v>
       </c>
       <c r="AK43" s="9">
-        <v>76.5</v>
+        <v>3</v>
       </c>
       <c r="AL43" s="7"/>
       <c r="AM43" s="7"/>
@@ -3479,7 +3502,7 @@
     </row>
     <row r="44" spans="1:41" ht="15.75" thickBot="1">
       <c r="A44" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44" s="9">
         <v>2</v>
@@ -3505,7 +3528,7 @@
         <v>2</v>
       </c>
       <c r="M44" s="9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N44" s="9">
         <v>15</v>
@@ -3513,45 +3536,45 @@
       <c r="O44" s="8"/>
       <c r="P44" s="8"/>
       <c r="Q44" s="9">
-        <v>98</v>
+        <v>63</v>
       </c>
       <c r="R44" s="8"/>
       <c r="S44" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T44" s="8"/>
-      <c r="U44" s="9">
-        <v>1</v>
-      </c>
-      <c r="V44" s="8"/>
+      <c r="U44" s="8"/>
+      <c r="V44" s="10">
+        <v>0</v>
+      </c>
       <c r="W44" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X44" s="9">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="Y44" s="8"/>
       <c r="Z44" s="12"/>
       <c r="AA44" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AB44" s="8"/>
       <c r="AC44" s="8"/>
       <c r="AD44" s="8"/>
-      <c r="AE44" s="10">
-        <v>57.5</v>
+      <c r="AE44" s="9">
+        <v>104</v>
       </c>
       <c r="AF44" s="9">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="AG44" s="8"/>
       <c r="AH44" s="8"/>
       <c r="AI44" s="8"/>
       <c r="AJ44" s="9">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AK44" s="9">
-        <v>73.5</v>
+        <v>76.5</v>
       </c>
       <c r="AL44" s="7"/>
       <c r="AM44" s="7"/>
@@ -3560,7 +3583,7 @@
     </row>
     <row r="45" spans="1:41" ht="15.75" thickBot="1">
       <c r="A45" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45" s="9">
         <v>2</v>
@@ -3593,40 +3616,46 @@
       </c>
       <c r="O45" s="8"/>
       <c r="P45" s="8"/>
-      <c r="Q45" s="8"/>
+      <c r="Q45" s="9">
+        <v>98</v>
+      </c>
       <c r="R45" s="8"/>
       <c r="S45" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T45" s="8"/>
-      <c r="U45" s="8"/>
+      <c r="U45" s="9">
+        <v>1</v>
+      </c>
       <c r="V45" s="8"/>
       <c r="W45" s="9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="X45" s="9">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="Y45" s="8"/>
       <c r="Z45" s="12"/>
-      <c r="AA45" s="8"/>
+      <c r="AA45" s="9">
+        <v>2</v>
+      </c>
       <c r="AB45" s="8"/>
       <c r="AC45" s="8"/>
       <c r="AD45" s="8"/>
-      <c r="AE45" s="9">
-        <v>32.5</v>
+      <c r="AE45" s="10">
+        <v>57.5</v>
       </c>
       <c r="AF45" s="9">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="AG45" s="8"/>
       <c r="AH45" s="8"/>
       <c r="AI45" s="8"/>
       <c r="AJ45" s="9">
-        <v>31</v>
+        <v>81</v>
       </c>
       <c r="AK45" s="9">
-        <v>29.5</v>
+        <v>73.5</v>
       </c>
       <c r="AL45" s="7"/>
       <c r="AM45" s="7"/>
@@ -3635,7 +3664,7 @@
     </row>
     <row r="46" spans="1:41" ht="15.75" thickBot="1">
       <c r="A46" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46" s="9">
         <v>2</v>
@@ -3677,10 +3706,10 @@
       <c r="U46" s="8"/>
       <c r="V46" s="8"/>
       <c r="W46" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="X46" s="9">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="Y46" s="8"/>
       <c r="Z46" s="12"/>
@@ -3689,7 +3718,7 @@
       <c r="AC46" s="8"/>
       <c r="AD46" s="8"/>
       <c r="AE46" s="9">
-        <v>30</v>
+        <v>32.5</v>
       </c>
       <c r="AF46" s="9">
         <v>25</v>
@@ -3697,18 +3726,20 @@
       <c r="AG46" s="8"/>
       <c r="AH46" s="8"/>
       <c r="AI46" s="8"/>
-      <c r="AJ46" s="8"/>
-      <c r="AK46" s="8"/>
-      <c r="AL46" s="9">
-        <v>12</v>
-      </c>
+      <c r="AJ46" s="9">
+        <v>31</v>
+      </c>
+      <c r="AK46" s="9">
+        <v>29.5</v>
+      </c>
+      <c r="AL46" s="7"/>
       <c r="AM46" s="7"/>
       <c r="AN46" s="7"/>
       <c r="AO46" s="8"/>
     </row>
     <row r="47" spans="1:41" ht="15.75" thickBot="1">
       <c r="A47" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47" s="9">
         <v>2</v>
@@ -3734,7 +3765,7 @@
         <v>2</v>
       </c>
       <c r="M47" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N47" s="9">
         <v>15</v>
@@ -3744,7 +3775,7 @@
       <c r="Q47" s="8"/>
       <c r="R47" s="8"/>
       <c r="S47" s="9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T47" s="8"/>
       <c r="U47" s="8"/>
@@ -3753,7 +3784,7 @@
         <v>3</v>
       </c>
       <c r="X47" s="9">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="Y47" s="8"/>
       <c r="Z47" s="12"/>
@@ -3762,28 +3793,26 @@
       <c r="AC47" s="8"/>
       <c r="AD47" s="8"/>
       <c r="AE47" s="9">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="AF47" s="9">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="AG47" s="8"/>
       <c r="AH47" s="8"/>
       <c r="AI47" s="8"/>
-      <c r="AJ47" s="9">
-        <v>32</v>
-      </c>
-      <c r="AK47" s="9">
-        <v>30.5</v>
-      </c>
-      <c r="AL47" s="7"/>
+      <c r="AJ47" s="8"/>
+      <c r="AK47" s="8"/>
+      <c r="AL47" s="9">
+        <v>12</v>
+      </c>
       <c r="AM47" s="7"/>
       <c r="AN47" s="7"/>
       <c r="AO47" s="8"/>
     </row>
     <row r="48" spans="1:41" ht="15.75" thickBot="1">
       <c r="A48" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B48" s="9">
         <v>2</v>
@@ -3808,8 +3837,8 @@
       <c r="L48" s="9">
         <v>2</v>
       </c>
-      <c r="M48" s="10">
-        <v>4</v>
+      <c r="M48" s="9">
+        <v>5</v>
       </c>
       <c r="N48" s="9">
         <v>15</v>
@@ -3825,7 +3854,7 @@
       <c r="U48" s="8"/>
       <c r="V48" s="8"/>
       <c r="W48" s="9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="X48" s="9">
         <v>12</v>
@@ -3837,24 +3866,99 @@
       <c r="AC48" s="8"/>
       <c r="AD48" s="8"/>
       <c r="AE48" s="9">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AF48" s="9">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="AG48" s="8"/>
       <c r="AH48" s="8"/>
       <c r="AI48" s="8"/>
-      <c r="AJ48" s="10">
-        <v>29</v>
+      <c r="AJ48" s="9">
+        <v>32</v>
       </c>
       <c r="AK48" s="9">
-        <v>29</v>
+        <v>30.5</v>
       </c>
       <c r="AL48" s="7"/>
       <c r="AM48" s="7"/>
       <c r="AN48" s="7"/>
       <c r="AO48" s="8"/>
+    </row>
+    <row r="49" spans="1:41" ht="15.75" thickBot="1">
+      <c r="A49" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B49" s="9">
+        <v>2</v>
+      </c>
+      <c r="C49" s="9">
+        <v>3</v>
+      </c>
+      <c r="D49" s="9">
+        <v>3</v>
+      </c>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="9">
+        <v>2</v>
+      </c>
+      <c r="K49" s="9">
+        <v>1</v>
+      </c>
+      <c r="L49" s="9">
+        <v>2</v>
+      </c>
+      <c r="M49" s="10">
+        <v>4</v>
+      </c>
+      <c r="N49" s="9">
+        <v>15</v>
+      </c>
+      <c r="O49" s="8"/>
+      <c r="P49" s="8"/>
+      <c r="Q49" s="8"/>
+      <c r="R49" s="8"/>
+      <c r="S49" s="9">
+        <v>1</v>
+      </c>
+      <c r="T49" s="8"/>
+      <c r="U49" s="8"/>
+      <c r="V49" s="8"/>
+      <c r="W49" s="9">
+        <v>1</v>
+      </c>
+      <c r="X49" s="9">
+        <v>12</v>
+      </c>
+      <c r="Y49" s="8"/>
+      <c r="Z49" s="12"/>
+      <c r="AA49" s="8"/>
+      <c r="AB49" s="8"/>
+      <c r="AC49" s="8"/>
+      <c r="AD49" s="8"/>
+      <c r="AE49" s="9">
+        <v>33</v>
+      </c>
+      <c r="AF49" s="9">
+        <v>18</v>
+      </c>
+      <c r="AG49" s="8"/>
+      <c r="AH49" s="8"/>
+      <c r="AI49" s="8"/>
+      <c r="AJ49" s="10">
+        <v>29</v>
+      </c>
+      <c r="AK49" s="9">
+        <v>29</v>
+      </c>
+      <c r="AL49" s="7"/>
+      <c r="AM49" s="7"/>
+      <c r="AN49" s="7"/>
+      <c r="AO49" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>